<commit_message>
added individuals and data properties
</commit_message>
<xml_diff>
--- a/AmplifiersData/OperationalAmplifiers.xlsx
+++ b/AmplifiersData/OperationalAmplifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vaibhavk/CS/Informatik/Thesis/Task1/AmplifiersData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24F6EBE-F93F-174D-8F71-72C735F02F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2F56FD-B26F-614D-98DB-9DB7A44035DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$AH$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$AH$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="83">
   <si>
     <t>Description</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Op Amp Dual Auto Zero Amplifier R-R I/O 5.5V Automotive 8-Pin SOIC N Tube None</t>
   </si>
   <si>
-    <t>Op Amp Dual Low Power Amplifier R-R I/O 24V 8-Pin PDIP Tube None</t>
-  </si>
-  <si>
     <t>Op Amp Dual GP R-R I/O 5.5V Automotive 8-Pin PDIP Tube None</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t xml:space="preserve">Auto Zero Amplifier </t>
   </si>
   <si>
-    <t xml:space="preserve">Low Power Amplifier </t>
-  </si>
-  <si>
     <t xml:space="preserve">General Purpose Amplifier </t>
   </si>
   <si>
@@ -167,9 +161,6 @@
     <t>MHz</t>
   </si>
   <si>
-    <t>3|5|9|12|15|18</t>
-  </si>
-  <si>
     <t>5|9|12|15</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
   </si>
   <si>
     <t xml:space="preserve">MCP6V27-E-SN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LM6132BIN-NOPB </t>
   </si>
   <si>
     <t xml:space="preserve">MCP6292-E-P </t>
@@ -701,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F286BF-E506-4741-97F8-48F53605C737}">
-  <dimension ref="A1:AH11"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="174" zoomScaleNormal="227" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="227" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -747,129 +735,129 @@
   <sheetData>
     <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3">
         <v>8</v>
@@ -878,102 +866,102 @@
         <v>80</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K2" s="3">
         <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M2" s="3">
         <v>6</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O2" s="3">
         <v>9</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S2" s="3">
         <v>2.5</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U2" s="3">
         <v>6</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="W2" s="3">
         <v>75</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA2" s="3">
         <v>-40</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC2" s="3">
         <v>85</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AE2" s="3">
         <v>30</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AG2" s="3">
         <v>0.155</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="3">
         <v>14</v>
@@ -982,102 +970,102 @@
         <v>70</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K3" s="3">
         <v>5.5</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M3" s="3">
         <v>5.5</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O3" s="3">
         <v>6</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S3" s="3">
         <v>1.8</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U3" s="3">
         <v>5.5</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="W3" s="3">
         <v>70</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y3" s="3">
         <v>1E-4</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA3" s="3">
         <v>-40</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC3" s="3">
         <v>125</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AE3" s="3">
         <v>30</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AG3" s="3">
         <v>0.01</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3">
         <v>8</v>
@@ -1086,301 +1074,301 @@
         <v>125</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K4" s="3">
         <v>5.5</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M4" s="3">
         <v>5.5</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O4" s="3">
         <v>6</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S4" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U4" s="3">
         <v>5.5</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="W4" s="3">
         <v>120</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA4" s="3">
         <v>-40</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC4" s="3">
         <v>125</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AE4" s="3">
         <v>30</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AG4" s="3">
         <v>2</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="3">
         <v>8</v>
       </c>
       <c r="I5" s="3">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="3">
+        <v>6</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="3">
-        <v>24</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="R5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5" s="3">
+        <v>6</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W5" s="3">
+        <v>70</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="Z5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="M5" s="3">
-        <v>17</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="3">
-        <v>30</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U5" s="3">
-        <v>24</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W5" s="3">
-        <v>60</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>0.18</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="AA5" s="3">
         <v>-40</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC5" s="3">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AE5" s="3">
         <v>30</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AG5" s="3">
         <v>10</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="3">
         <v>8</v>
       </c>
       <c r="I6" s="3">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K6" s="3">
         <v>5.5</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M6" s="3">
         <v>5.5</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O6" s="3">
         <v>6</v>
       </c>
       <c r="P6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U6" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W6" s="3">
+        <v>120</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z6" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S6" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U6" s="3">
-        <v>6</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W6" s="3">
-        <v>70</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="AA6" s="3">
         <v>-40</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC6" s="3">
         <v>125</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AE6" s="3">
         <v>30</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AG6" s="3">
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
@@ -1395,290 +1383,290 @@
         <v>8</v>
       </c>
       <c r="I7" s="3">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="3">
-        <v>5.5</v>
+        <v>34</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M7" s="3">
         <v>5.5</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O7" s="3">
         <v>6</v>
       </c>
       <c r="P7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="3">
+        <v>3</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" s="3">
+        <v>12</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W7" s="3">
+        <v>72</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="Z7" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S7" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U7" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W7" s="3">
-        <v>120</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z7" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="AA7" s="3">
         <v>-40</v>
       </c>
       <c r="AB7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>85</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>110</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>86</v>
+      </c>
+      <c r="AH7" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>125</v>
-      </c>
-      <c r="AD7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE7" s="3">
-        <v>30</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG7" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="AH7" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="3">
         <v>8</v>
       </c>
       <c r="I8" s="3">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="3">
+        <v>12</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="R8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="3">
+        <v>4</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U8" s="3">
+        <v>40</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8" s="3">
+        <v>85</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z8" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="M8" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O8" s="3">
-        <v>6</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S8" s="3">
-        <v>3</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U8" s="3">
-        <v>12</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W8" s="3">
-        <v>72</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="AA8" s="3">
         <v>-40</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC8" s="3">
         <v>85</v>
       </c>
       <c r="AD8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>20</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AH8" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="AE8" s="3">
-        <v>110</v>
-      </c>
-      <c r="AF8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG8" s="3">
-        <v>86</v>
-      </c>
-      <c r="AH8" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3">
         <v>8</v>
       </c>
-      <c r="I9" s="3">
-        <v>72</v>
+      <c r="I9" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
+      </c>
+      <c r="K9" s="3">
+        <v>16</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="3">
+        <v>16</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="3">
+        <v>17</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>3</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U9" s="3">
+        <v>5</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W9" s="3">
+        <v>54</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z9" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="M9" s="3">
-        <v>12</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O9" s="3">
-        <v>12.5</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S9" s="3">
-        <v>4</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U9" s="3">
-        <v>40</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W9" s="3">
-        <v>85</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y9" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="AA9" s="3">
         <v>-40</v>
       </c>
       <c r="AB9" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC9" s="3">
         <v>85</v>
       </c>
       <c r="AD9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="AH9" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="AE9" s="3">
-        <v>20</v>
-      </c>
-      <c r="AF9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="AH9" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
@@ -1689,16 +1677,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>22</v>
@@ -1706,192 +1694,88 @@
       <c r="H10" s="3">
         <v>8</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>58</v>
+      <c r="I10" s="3">
+        <v>87.96</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K10" s="3">
+        <v>5</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U10" s="3">
         <v>16</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="V10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W10" s="3">
+        <v>70</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="Z10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M10" s="3">
-        <v>16</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O10" s="3">
-        <v>17</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>3</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S10" s="3">
-        <v>2.7</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U10" s="3">
-        <v>5</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W10" s="3">
+      <c r="AA10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="X10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y10" s="3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AB10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>70</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>50</v>
+      </c>
+      <c r="AF10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AA10" s="3">
-        <v>-40</v>
-      </c>
-      <c r="AB10" s="3" t="s">
+      <c r="AG10" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="AH10" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="AC10" s="3">
-        <v>85</v>
-      </c>
-      <c r="AD10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG10" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="AH10" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="3">
-        <v>8</v>
-      </c>
-      <c r="I11" s="3">
-        <v>87.96</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="3">
-        <v>5</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S11" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U11" s="3">
-        <v>16</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W11" s="3">
-        <v>70</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y11" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC11" s="3">
-        <v>70</v>
-      </c>
-      <c r="AD11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE11" s="3">
-        <v>50</v>
-      </c>
-      <c r="AF11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG11" s="3">
-        <v>0.71</v>
-      </c>
-      <c r="AH11" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH11" xr:uid="{E8F286BF-E506-4741-97F8-48F53605C737}"/>
-  <conditionalFormatting sqref="A1:AH11">
+  <autoFilter ref="A1:AH10" xr:uid="{E8F286BF-E506-4741-97F8-48F53605C737}"/>
+  <conditionalFormatting sqref="A1:AH10">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>

</xml_diff>